<commit_message>
A1-A7 task evidence format is incorrect UPDATE
</commit_message>
<xml_diff>
--- a/secard51/evidence.xlsx
+++ b/secard51/evidence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SECARD\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92099D8-5FA9-4A79-BE84-50DAEA103DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C342C661-B543-4BEA-A6B6-D4FC63FC635B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="41">
   <si>
     <t>TeamName</t>
   </si>
@@ -93,12 +93,6 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
     <t>tx hash on that chain</t>
   </si>
   <si>
@@ -159,18 +153,9 @@
     <t>uni-6</t>
   </si>
   <si>
-    <t>contract : juno1ngjawawweu8w3x0ttc8ygkajj73ek6k8x4um92w00wgd9dvnfrvqryq20v</t>
-  </si>
-  <si>
-    <t>class id : wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-89/paloma</t>
-  </si>
-  <si>
     <t>7CBF01C742A7C2EBC3A01F2A7EB3ED7276B412FA6868A3FEBBDFF656789DE8EB</t>
   </si>
   <si>
-    <t>gon-irishub-1</t>
-  </si>
-  <si>
     <t>0C1AC6D12837B70ACD16A1788D049DCE29C85DFBD6366152DB588DF53EEFAF2B</t>
   </si>
   <si>
@@ -186,13 +171,13 @@
     <t>gon-flixnet-1</t>
   </si>
   <si>
-    <t>collection:ibc/80EEB74FA4B834313769C43A2AE8B498CB1B5A429FFA0511B053E47247726ACF</t>
-  </si>
-  <si>
-    <t>class id : nft-transfer/channel-24/paloma</t>
-  </si>
-  <si>
     <t>DED08AA020D8CDEA534B046E77C6BC5B143AED2F36DF0CD38F34ECDABFDAB09F</t>
+  </si>
+  <si>
+    <t>ibc/B8A601CB661FF86E40CD428AF78251DCCAFC580374909EF9FFF47B0FD405E53A</t>
+  </si>
+  <si>
+    <t>secardnft1</t>
   </si>
 </sst>
 </file>
@@ -655,28 +640,28 @@
     </row>
     <row r="2" spans="1:8" ht="13.8">
       <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -689,7 +674,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
@@ -705,12 +692,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -722,7 +705,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
@@ -738,12 +723,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -755,7 +736,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
@@ -771,12 +754,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -788,7 +767,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
@@ -804,12 +785,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -821,7 +798,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
@@ -838,20 +817,20 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -881,20 +860,20 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -924,20 +903,20 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -967,20 +946,20 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1010,20 +989,20 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1053,20 +1032,20 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1099,10 +1078,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1132,20 +1111,20 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1175,20 +1154,20 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1212,12 +1191,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1247,12 +1226,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.8">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1282,12 +1261,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.8">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1317,12 +1296,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.8">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1362,24 +1341,24 @@
     </row>
     <row r="2" spans="1:3" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1390,7 +1369,55 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="13.8">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="13.8">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4:J5"/>
@@ -1418,40 +1445,30 @@
     </row>
     <row r="2" spans="1:4" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D5"/>
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:J5"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -1476,84 +1493,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="D4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
-  <cols>
-    <col min="1" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="13.8">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="13.8">
-      <c r="A2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="D5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1564,10 +1513,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -1594,26 +1543,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="D4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="D5" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1626,11 +1565,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
-  <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="37.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="13.8">
@@ -1643,10 +1584,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1659,7 +1600,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="A2:C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
@@ -1675,12 +1618,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
A1-A7 task evidence format is incorrect reUPDATE
</commit_message>
<xml_diff>
--- a/secard51/evidence.xlsx
+++ b/secard51/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SECARD\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1584F19F-EE00-485E-AED4-1CD5E0EEB9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737635F0-E599-4C4A-943C-EFBB26D09001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="41">
   <si>
     <t>TeamName</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>BE33EC482B11740D13CB6AEB64485D940B69514D5BD483E98517C940B4F7B5EB</t>
-  </si>
-  <si>
-    <t>wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-89/paloma</t>
   </si>
   <si>
     <t>uni-6</t>
@@ -708,7 +705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -1344,13 +1341,13 @@
     </row>
     <row r="2" spans="1:3" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="13.8">
@@ -1403,13 +1400,13 @@
         <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1448,16 +1445,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.8">
       <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1470,8 +1467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -1496,16 +1493,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1546,16 +1543,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1587,10 +1584,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A1-A20 Stage2 Evidence UPDATE
</commit_message>
<xml_diff>
--- a/secard51/evidence.xlsx
+++ b/secard51/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SECARD\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737635F0-E599-4C4A-943C-EFBB26D09001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0091CF9-4AEA-4ED7-823E-052EB7F7D08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="588" firstSheet="7" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="87">
   <si>
     <t>TeamName</t>
   </si>
@@ -93,15 +93,6 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
   </si>
   <si>
@@ -153,6 +144,9 @@
     <t>7CBF01C742A7C2EBC3A01F2A7EB3ED7276B412FA6868A3FEBBDFF656789DE8EB</t>
   </si>
   <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
     <t>0C1AC6D12837B70ACD16A1788D049DCE29C85DFBD6366152DB588DF53EEFAF2B</t>
   </si>
   <si>
@@ -177,14 +171,158 @@
     <t>secardnft1</t>
   </si>
   <si>
+    <t>ibc/ACD5BB81990F758D6C72B87429F96DB9FC421F74C3181285F2F415AB2BA19693</t>
+  </si>
+  <si>
+    <t>secardnft2</t>
+  </si>
+  <si>
+    <t>ibc/64A93C867576BAEBC2A19CD2D580E34D449C4D125DCBD7096C6073B000E31393</t>
+  </si>
+  <si>
+    <t>secardnft4</t>
+  </si>
+  <si>
+    <t>ibc/14AB93E7AB494FEEF700DC23E371C846646BB8C4EE828FB93C0BA4726130D44F</t>
+  </si>
+  <si>
+    <t>secardnft5</t>
+  </si>
+  <si>
+    <t>ibc/2385F62B94D68390640C59C57B0623310B550A47D9339DE759BC67B454799BE7</t>
+  </si>
+  <si>
+    <t>secardnft6</t>
+  </si>
+  <si>
+    <t>ibc/C9BBCE327ECD739390CEDDBFDCD239A86C1650EA7B4467A79C0645903C88C682</t>
+  </si>
+  <si>
+    <t>secardnft8</t>
+  </si>
+  <si>
     <t>juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-89/paloma</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>68DBC540EAA0E4253D7C7F70CFB9FB8D2C232B6496833DB429432B1446E102D2</t>
+  </si>
+  <si>
+    <t>F94529E25D80F3319F71DFE767D06F52829F204E79FDDFEA7A3757EE42C4E515</t>
+  </si>
+  <si>
+    <t>6EC23F317D5759854F0613A3944D8E3CF9AF8045A0F33287368D54722CF5A549</t>
+  </si>
+  <si>
+    <t>80F9D2AFFF939D798D3BA9287491780ADAC655C7EB5106AAF5E2101B83D11D5E</t>
+  </si>
+  <si>
+    <t>60E2D539EECE785FCD25399501837945FF13FE3FBF05590DAEA78C6621AE4830</t>
+  </si>
+  <si>
+    <t>33C60E73DE113332D866C15CBA6EAC50CAD30E5008B66D83D92CCFB70DA92BF8</t>
+  </si>
+  <si>
+    <t>5F32348AF82DA0921D7A41C38AE8961D650AE047CEC00E874B05712C8E8C7242</t>
+  </si>
+  <si>
+    <t>A6A98A682C0FF8E4F2A305CBDDA8D3A0839B6525C43C85EEF8F4E0746FEFAAFB</t>
+  </si>
+  <si>
+    <t>4B9D515E3D07F9700AC8CD2905846E45421B4A0667338A63C061A3165348E5D9</t>
+  </si>
+  <si>
+    <t>6DAD05FDE1D6CD5C0C6F543E24B425804C8CDA74E87F036F85127E1A06451B60</t>
+  </si>
+  <si>
+    <t>65DA9A00334094EFD4DDA82D950D7ECCFB78DD46AB6AAF71368B79170040BE68</t>
+  </si>
+  <si>
+    <t>52359463F4BBB85214A8C8EB370391CC889468C9B7D563D33BE594B6D095F7B0</t>
+  </si>
+  <si>
+    <t>33A57EE16D2B49C2011D4B673B7ACFDE46D06AFC7389478880206655F21EDC9B</t>
+  </si>
+  <si>
+    <t>C17A40004014C9C2A55A6206FA8BC76EF6F62F42C0A5D3E78A623EB193F91359</t>
+  </si>
+  <si>
+    <t>4051372135B9023BFFEFB2C918544AB3DF313CA00F4331955A4D790788BB34D2</t>
+  </si>
+  <si>
+    <t>E38C75B88F4F9A72A4BF3444536AC625E6E32A92981963939D1CCDF615EDC656</t>
+  </si>
+  <si>
+    <t>6A8C34D244D6BFFA3C946256871BECCAE80D4580E68A3420F2CD06B287E15B8E</t>
+  </si>
+  <si>
+    <t>ED1A81B257C551368B56A3E0DC3FFDC3CEAD88960E0DF3AD57F6F233B7881E2F</t>
+  </si>
+  <si>
+    <t>117D316731282155CD138508C669BF40F256B117170D19673F8AA4752BBFD328</t>
+  </si>
+  <si>
+    <t>C83E57DCDF20DF22198A9C96301F887CEA048245DFCA1EE48AF3C95CBFF1F91B</t>
+  </si>
+  <si>
+    <t>C7BC84A620D948202F2A779C9BA4305F84C9EF0C6A7D3C45DAE05725361D5E72</t>
+  </si>
+  <si>
+    <t>B9EFA24F776D884C88B43077A32B4696FFD32A22BD37EFA197A399E799D7756E</t>
+  </si>
+  <si>
+    <t>63B7B9C4A3A5669EB6928B0BBDA7E10C3F60D4660406C055FADF8E850382C36E</t>
+  </si>
+  <si>
+    <t>6605A54DA0488883D67124B4D9926356E0D7FC6FE0CA71FB74EF4087FA18CFFE</t>
+  </si>
+  <si>
+    <t>F0555A7642B728F42F7C8D16E69F2FD92D107814DA97617A364D72617947212C</t>
+  </si>
+  <si>
+    <t>965474B43AA56B34D115BF3969A53187FB7E1EAD4423D8DAF3CE1165A3597961</t>
+  </si>
+  <si>
+    <t>9554A7EF038DDD743BCC5E2D6B34B0AECBACDA797CDECC73A7F4E03F6453A79A</t>
+  </si>
+  <si>
+    <t>ED60BB0E599BC3A8590487C9D208816308C75FAF0C68995408AD2177D376F729</t>
+  </si>
+  <si>
+    <t>9807EC1BCCD9011E367BFC9FA72777275884F40799E7CA870A56EFD4A49B558C</t>
+  </si>
+  <si>
+    <t>D5B029BFE549494087A61BFB03E3AF5A732F60C4E14E7D3E5214F4FF3708899D</t>
+  </si>
+  <si>
+    <t>C8DF1CBF47107DD30F0A720386EBEE45E232FD0043355C1A3120B5CAEBC11F5F</t>
+  </si>
+  <si>
+    <t>90A809F8A150E60509208ACA3937E61D488CFA9C08C796DDCB2280A6D8D96509</t>
+  </si>
+  <si>
+    <t>9F00422AC0B43900C7EDD59606D54441BD23FFB47EF08413059113A4C951D223</t>
+  </si>
+  <si>
+    <t>2B6669593D20903D4F34324C788BFF90A27E6DD23CACADC63869DDC8A631BA7E</t>
+  </si>
+  <si>
+    <t>4C208292B2823CBA8A865A7187EB7F8C1DDE2E5EC11E8066CD127F3E73ED0B7F</t>
+  </si>
+  <si>
+    <t>A0E0187E67AE99C1E0713E1A10AAC8C0B9AF11B3054E678BD17497477B4CC16A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -209,6 +347,26 @@
       <color theme="10"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
     </font>
   </fonts>
   <fills count="4">
@@ -244,13 +402,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -640,28 +806,28 @@
     </row>
     <row r="2" spans="1:8" ht="13.8">
       <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -675,7 +841,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -692,8 +858,12 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -706,7 +876,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -723,8 +893,12 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -737,7 +911,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -754,8 +928,12 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -768,7 +946,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -785,8 +963,12 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -796,10 +978,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="A2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -817,20 +999,34 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -841,9 +1037,11 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
@@ -859,21 +1057,35 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
+      <c r="A2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
+      <c r="A3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
+      <c r="A4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -884,9 +1096,11 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
@@ -902,21 +1116,35 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
+      <c r="A2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
+      <c r="A3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
+      <c r="A4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -927,9 +1155,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
@@ -945,21 +1175,35 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
+      <c r="A2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
+      <c r="A3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
+      <c r="A4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -970,9 +1214,11 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
@@ -988,21 +1234,35 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
+      <c r="A2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
+      <c r="A3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
+      <c r="A4" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1013,9 +1273,11 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
@@ -1031,21 +1293,35 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
+      <c r="A2" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
+      <c r="A3" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
+      <c r="A4" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13.8">
+      <c r="A5" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1064,8 +1340,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="38.109375" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="1" max="2" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="13.8">
@@ -1078,10 +1353,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1092,9 +1367,86 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.8">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="13.8">
+      <c r="A2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="13.8">
+      <c r="A3" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="13.8">
+      <c r="A4" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
   <cols>
@@ -1111,63 +1463,50 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>81</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
-  <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="13.8">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="13.8">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="13.8">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1191,12 +1530,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1226,12 +1565,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.8">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1261,12 +1600,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.8">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1296,12 +1635,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.8">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1341,24 +1680,24 @@
     </row>
     <row r="2" spans="1:3" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1372,7 +1711,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -1397,16 +1736,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1445,16 +1784,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.8">
       <c r="A2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1467,8 +1806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -1493,16 +1832,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1516,7 +1855,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="L10" sqref="D4:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -1543,16 +1882,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1566,12 +1905,47 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
-  <cols>
-    <col min="1" max="1" width="37.21875" customWidth="1"/>
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.8">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="13.8">
+      <c r="A2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="13.8">
@@ -1592,37 +1966,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
-  <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="13.8">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
A3-A5-A6 UPDATE A18 ?
I didn't see any problem in A18
</commit_message>
<xml_diff>
--- a/secard51/evidence.xlsx
+++ b/secard51/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SECARD\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GNS\Desktop\arda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DAFE74-0253-4A22-AFE4-F23C8150C8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835621CB-A4BD-4DA9-9761-03929BBF1D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="588" firstSheet="7" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="588" firstSheet="5" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -201,9 +201,6 @@
     <t>secardnft8</t>
   </si>
   <si>
-    <t>juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-89/paloma</t>
-  </si>
-  <si>
     <t>elgafar-1</t>
   </si>
   <si>
@@ -328,18 +325,28 @@
   </si>
   <si>
     <t>C97D3A4C8799A15F6E5A234DF80B3E25E9025CC3022527410DE885D718877EEC</t>
+  </si>
+  <si>
+    <t>juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -410,29 +417,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{5919E0D2-0BDF-40E7-BAF6-73E660F41B63}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1011,7 +1024,7 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>
@@ -1019,26 +1032,26 @@
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1070,7 +1083,7 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>29</v>
@@ -1078,15 +1091,15 @@
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -1094,10 +1107,10 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1129,7 +1142,7 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>29</v>
@@ -1137,7 +1150,7 @@
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -1145,15 +1158,15 @@
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
@@ -1188,7 +1201,7 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>29</v>
@@ -1196,7 +1209,7 @@
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -1204,15 +1217,15 @@
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
@@ -1247,7 +1260,7 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>29</v>
@@ -1255,15 +1268,15 @@
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
@@ -1271,10 +1284,10 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1287,13 +1300,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
-  <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="102.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="13.8">
@@ -1306,7 +1319,7 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>29</v>
@@ -1314,7 +1327,7 @@
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>34</v>
@@ -1322,15 +1335,15 @@
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13.8">
+      <c r="A5" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="13.8">
-      <c r="A5" s="8" t="s">
-        <v>74</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>34</v>
@@ -1338,7 +1351,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1400,7 +1413,7 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>29</v>
@@ -1408,15 +1421,15 @@
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
@@ -1424,15 +1437,15 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
@@ -1440,10 +1453,10 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1475,7 +1488,7 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>29</v>
@@ -1483,23 +1496,23 @@
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
@@ -1507,18 +1520,18 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1531,7 +1544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1544,12 +1557,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1579,12 +1592,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.8">
       <c r="A2" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1725,7 +1738,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -1753,7 +1766,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>25</v>
@@ -1849,7 +1862,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>25</v>
@@ -1869,7 +1882,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="D4:L10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -1904,8 +1917,8 @@
       <c r="C2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>29</v>
+      <c r="D2" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>